<commit_message>
add on parse call back.
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cny/go/src/github.com/codingeasygo/xlsx2json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7C9EDD-D44B-7941-9A91-17ECDFF1A3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEE8FF9-6091-904B-A742-8A8FE0D40A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="2200" windowWidth="28580" windowHeight="25300" activeTab="1" xr2:uid="{1D59D8A5-CF87-F042-9C22-F01DDD5C7962}"/>
+    <workbookView xWindow="14680" yWindow="2200" windowWidth="28580" windowHeight="25300" activeTab="2" xr2:uid="{1D59D8A5-CF87-F042-9C22-F01DDD5C7962}"/>
   </bookViews>
   <sheets>
     <sheet name="user0" sheetId="1" r:id="rId1"/>
     <sheet name="user1" sheetId="3" r:id="rId2"/>
-    <sheet name="product" sheetId="2" r:id="rId3"/>
+    <sheet name="user2" sheetId="4" r:id="rId3"/>
+    <sheet name="product" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>id,int64</t>
   </si>
@@ -131,6 +132,10 @@
   </si>
   <si>
     <t>products_3,ref,product,test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a,xxx</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -617,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB5166C-9824-0047-80FD-31E10BA46393}">
   <dimension ref="A2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -662,6 +667,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233265DC-6DA8-8E45-B207-3BECE4A665D1}">
+  <dimension ref="A2:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="43.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC002A4A-8418-7F42-9C70-06C000837661}">
   <dimension ref="A2:G4"/>
   <sheetViews>

</xml_diff>